<commit_message>
chapter complete 2D case analysis and 3D case begin
</commit_message>
<xml_diff>
--- a/xjh/TEST/Onera/postprocess.xlsx
+++ b/xjh/TEST/Onera/postprocess.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xjh/thesis/xjh/TEST/Onera/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6BE61C-C17C-2242-8D21-141FDEB69A42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420C1E46-A89F-2C4A-A590-8C01B0A4C0A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{E813E3D2-8B92-5C49-8DD6-185F646B6F3F}"/>
   </bookViews>
@@ -571,7 +571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BEE77C-FC9B-2A4B-B70C-ACB86D236C97}">
   <dimension ref="A1:BP256"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="83" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView topLeftCell="H28" zoomScale="83" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="P54" sqref="P54"/>
     </sheetView>
   </sheetViews>
@@ -8834,8 +8834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E60AECBB-FA79-814B-BF8F-04A58F7DEA5D}">
   <dimension ref="A1:AA137"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:O54"/>
+    <sheetView topLeftCell="D1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11579,8 +11579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01678F02-6852-1843-B1D7-578F6A92EC72}">
   <dimension ref="A1:U155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F17" zoomScale="117" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:O54"/>
+    <sheetView tabSelected="1" topLeftCell="H38" zoomScale="117" zoomScaleNormal="58" workbookViewId="0">
+      <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>